<commit_message>
Integrate Agora data for buildings sector vars BDEQ, RBFF, and FoBObE
</commit_message>
<xml_diff>
--- a/InputData/bldgs/RBFF/Recipient Buildings Fuel Fractions.xlsx
+++ b/InputData/bldgs/RBFF/Recipient Buildings Fuel Fractions.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipD\InputData\bldgs\RBFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Desktop\PhD\EPS\InputData_new\bldgs\RBFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="11295"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25812" windowHeight="11292"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RBFF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,12 +51,6 @@
     <t>for the buildings fuel shifting policy.  It is used</t>
   </si>
   <si>
-    <t>For the U.S. model, it is configured to shift all fuels to</t>
-  </si>
-  <si>
-    <t>electricity.</t>
-  </si>
-  <si>
     <t>To type (below)  / From type (right)</t>
   </si>
   <si>
@@ -91,12 +85,18 @@
   </si>
   <si>
     <t>Ensure that every column adds to 1.</t>
+  </si>
+  <si>
+    <t>For the EU model, we assume that fossil boilers are replaced by heat pumps and district heating</t>
+  </si>
+  <si>
+    <t>in equal shares. Further we assume that biomass boilers are replaced with biomass.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,7 +152,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -432,16 +432,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -449,44 +451,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -502,368 +504,370 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="6" width="17.28515625" style="5" customWidth="1"/>
-    <col min="7" max="11" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="6" width="17.33203125" style="5" customWidth="1"/>
+    <col min="7" max="11" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="5">
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
-      <c r="H2" s="5">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5">
-        <v>1</v>
-      </c>
-      <c r="J2" s="5">
-        <v>1</v>
-      </c>
-      <c r="K2" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>

</xml_diff>